<commit_message>
add Generic in product
</commit_message>
<xml_diff>
--- a/public/file/template_upload_new_other_product.xlsx
+++ b/public/file/template_upload_new_other_product.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Price</t>
   </si>
@@ -33,6 +33,9 @@
   </si>
   <si>
     <t>Satuan</t>
+  </si>
+  <si>
+    <t>Generik</t>
   </si>
 </sst>
 </file>
@@ -361,7 +364,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C1"/>
+  <dimension ref="A1:D1"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -373,7 +376,7 @@
     <col min="2" max="2" width="8.5" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>1</v>
       </c>
@@ -383,6 +386,9 @@
       <c r="C1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>